<commit_message>
fix bug exeded requeste in google drive
</commit_message>
<xml_diff>
--- a/Listas de precios/mayorista/TANQUE.xlsx
+++ b/Listas de precios/mayorista/TANQUE.xlsx
@@ -775,7 +775,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="21" t="n">
-        <v>45309</v>
+        <v>45311</v>
       </c>
     </row>
     <row r="6" ht="22.5" customHeight="1" s="13">
@@ -2148,8 +2148,8 @@
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B107:C107"/>
     <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B88:C88"/>
     <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B88:C88"/>
     <mergeCell ref="B82:C82"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B34:C34"/>

</xml_diff>